<commit_message>
Se agrega dashboard de Sales
</commit_message>
<xml_diff>
--- a/front-dataflowai/public/plantillas-dashboards/4.xlsx
+++ b/front-dataflowai/public/plantillas-dashboards/4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coltradecomco-my.sharepoint.com/personal/tecnologia_coltrade_com_co/Documents/Coltrade/BUSINESS INTELLIGENCE/02. AREAS/DATA/Julian Estif Herreno Palacios/09-DataFlow-WebSite/front-dataflowai/src/assets/plantillas-dashboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E8CAF1-1ECD-47A9-9FF4-5C01C7B41B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B5FCFB-D9BC-4862-8AA0-AB784D320576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,48 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
-  <si>
-    <t>id_punto_venta</t>
-  </si>
-  <si>
-    <t>punto_venta</t>
-  </si>
-  <si>
-    <t>canal</t>
-  </si>
-  <si>
-    <t>ciudad</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>cantidad_vendida</t>
-  </si>
-  <si>
-    <t>dinero_vendido</t>
-  </si>
-  <si>
-    <t>ticket_promedio</t>
-  </si>
-  <si>
-    <t>unidades_promocionadas</t>
-  </si>
-  <si>
-    <t>descuento_total</t>
-  </si>
-  <si>
-    <t>numero_transacciones</t>
-  </si>
-  <si>
-    <t>devoluciones</t>
-  </si>
-  <si>
-    <t>dinero_devoluciones</t>
-  </si>
-  <si>
-    <t>fecha_venta</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>fecha_registro</t>
   </si>
   <si>
     <t>mes</t>
@@ -70,100 +31,76 @@
     <t>anio</t>
   </si>
   <si>
-    <t>dia_semana</t>
-  </si>
-  <si>
-    <t>hora</t>
-  </si>
-  <si>
-    <t>sku</t>
-  </si>
-  <si>
-    <t>nombre_producto</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>subcategoria</t>
-  </si>
-  <si>
-    <t>marca</t>
-  </si>
-  <si>
-    <t>tipo_cliente</t>
-  </si>
-  <si>
-    <t>segmento_cliente</t>
-  </si>
-  <si>
-    <t>genero_cliente</t>
-  </si>
-  <si>
-    <t>edad_cliente</t>
+    <t>ingresos_operacionales</t>
+  </si>
+  <si>
+    <t>ingresos_no_operacionales</t>
+  </si>
+  <si>
+    <t>ingresos_totales</t>
+  </si>
+  <si>
+    <t>costo_ventas</t>
+  </si>
+  <si>
+    <t>gastos_operacionales</t>
+  </si>
+  <si>
+    <t>otros_gastos</t>
+  </si>
+  <si>
+    <t>total_egresos</t>
   </si>
   <si>
     <t>utilidad_bruta</t>
   </si>
   <si>
-    <t>costo_total</t>
-  </si>
-  <si>
-    <t>margen_utilidad</t>
+    <t>utilidad_neta</t>
+  </si>
+  <si>
+    <t>margen_neto</t>
+  </si>
+  <si>
+    <t>flujo_efectivo_operaciones</t>
+  </si>
+  <si>
+    <t>flujo_efectivo_inversion</t>
+  </si>
+  <si>
+    <t>flujo_efectivo_financiacion</t>
+  </si>
+  <si>
+    <t>flujo_efectivo_total</t>
+  </si>
+  <si>
+    <t>activos_totales</t>
+  </si>
+  <si>
+    <t>pasivos_totales</t>
+  </si>
+  <si>
+    <t>patrimonio</t>
   </si>
   <si>
     <t>observaciones</t>
   </si>
   <si>
-    <t>PV-001</t>
-  </si>
-  <si>
-    <t>Tienda Física</t>
-  </si>
-  <si>
-    <t>Bogotá</t>
-  </si>
-  <si>
-    <t>Cundinamarca</t>
-  </si>
-  <si>
-    <t>2025-07-28</t>
-  </si>
-  <si>
-    <t>Lunes</t>
-  </si>
-  <si>
-    <t>14:30:00</t>
-  </si>
-  <si>
-    <t>SKU-12345</t>
-  </si>
-  <si>
-    <t>Smartphone X</t>
-  </si>
-  <si>
-    <t>Electrónicos</t>
-  </si>
-  <si>
-    <t>Telefonía</t>
-  </si>
-  <si>
-    <t>MarcaTech</t>
-  </si>
-  <si>
-    <t>Minorista</t>
-  </si>
-  <si>
-    <t>Consumo General</t>
-  </si>
-  <si>
-    <t>Femenino</t>
-  </si>
-  <si>
-    <t>Venta especial con descuento por lanzamiento</t>
-  </si>
-  <si>
-    <t>Julipan</t>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>2025-06-30</t>
+  </si>
+  <si>
+    <t>2025-05-31</t>
+  </si>
+  <si>
+    <t>Cierre financiero del segundo trimestre con resultados positivos.</t>
+  </si>
+  <si>
+    <t>Resultados del primer semestre con buen margen.</t>
+  </si>
+  <si>
+    <t>Mes con leve caída en ingresos no operacionales.</t>
   </si>
 </sst>
 </file>
@@ -233,7 +170,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{C426A3BC-5E3A-4962-8A2B-B32804AA2691}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{08FF1510-42AB-4617-9B99-9D8F3C0F0906}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -533,46 +470,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="59.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,130 +562,200 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>2025</v>
+      </c>
+      <c r="D2">
+        <v>15000000</v>
+      </c>
+      <c r="E2">
+        <v>2500000</v>
+      </c>
+      <c r="F2">
+        <v>17500000</v>
+      </c>
+      <c r="G2">
+        <v>7000000</v>
+      </c>
+      <c r="H2">
+        <v>3000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000</v>
+      </c>
+      <c r="J2">
+        <v>11000000</v>
+      </c>
+      <c r="K2">
+        <v>8000000</v>
+      </c>
+      <c r="L2">
+        <v>6500000</v>
+      </c>
+      <c r="M2">
+        <v>37.14</v>
+      </c>
+      <c r="N2">
+        <v>4000000</v>
+      </c>
+      <c r="O2">
+        <v>-500000</v>
+      </c>
+      <c r="P2">
+        <v>2000000</v>
+      </c>
+      <c r="Q2">
+        <v>5500000</v>
+      </c>
+      <c r="R2">
+        <v>32000000</v>
+      </c>
+      <c r="S2">
+        <v>12000000</v>
+      </c>
+      <c r="T2">
+        <v>20000000</v>
+      </c>
+      <c r="U2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2025</v>
+      </c>
+      <c r="D3">
+        <v>13000000</v>
+      </c>
+      <c r="E3">
+        <v>2000000</v>
+      </c>
+      <c r="F3">
+        <v>15000000</v>
+      </c>
+      <c r="G3">
+        <v>6000000</v>
+      </c>
+      <c r="H3">
+        <v>2500000</v>
+      </c>
+      <c r="I3">
+        <v>500000</v>
+      </c>
+      <c r="J3">
+        <v>9000000</v>
+      </c>
+      <c r="K3">
+        <v>7000000</v>
+      </c>
+      <c r="L3">
+        <v>6000000</v>
+      </c>
+      <c r="M3">
+        <v>40</v>
+      </c>
+      <c r="N3">
+        <v>3500000</v>
+      </c>
+      <c r="O3">
+        <v>-300000</v>
+      </c>
+      <c r="P3">
+        <v>1800000</v>
+      </c>
+      <c r="Q3">
+        <v>5000000</v>
+      </c>
+      <c r="R3">
+        <v>31000000</v>
+      </c>
+      <c r="S3">
+        <v>11000000</v>
+      </c>
+      <c r="T3">
+        <v>20000000</v>
+      </c>
+      <c r="U3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2025</v>
+      </c>
+      <c r="D4">
+        <v>14000000</v>
+      </c>
+      <c r="E4">
+        <v>1000000</v>
+      </c>
+      <c r="F4">
+        <v>15000000</v>
+      </c>
+      <c r="G4">
+        <v>6500000</v>
+      </c>
+      <c r="H4">
+        <v>2800000</v>
+      </c>
+      <c r="I4">
+        <v>700000</v>
+      </c>
+      <c r="J4">
+        <v>10000000</v>
+      </c>
+      <c r="K4">
+        <v>7500000</v>
+      </c>
+      <c r="L4">
+        <v>5000000</v>
+      </c>
+      <c r="M4">
+        <v>33.33</v>
+      </c>
+      <c r="N4">
+        <v>3000000</v>
+      </c>
+      <c r="O4">
+        <v>-400000</v>
+      </c>
+      <c r="P4">
+        <v>1500000</v>
+      </c>
+      <c r="Q4">
+        <v>4100000</v>
+      </c>
+      <c r="R4">
+        <v>29000000</v>
+      </c>
+      <c r="S4">
+        <v>10000000</v>
+      </c>
+      <c r="T4">
+        <v>19000000</v>
+      </c>
+      <c r="U4" t="s">
         <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2">
-        <v>120</v>
-      </c>
-      <c r="G2">
-        <v>56000000</v>
-      </c>
-      <c r="H2">
-        <v>37500</v>
-      </c>
-      <c r="I2">
-        <v>30</v>
-      </c>
-      <c r="J2">
-        <v>150000</v>
-      </c>
-      <c r="K2">
-        <v>115</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>200000</v>
-      </c>
-      <c r="N2" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2">
-        <v>7</v>
-      </c>
-      <c r="P2">
-        <v>2025</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
-      </c>
-      <c r="U2" t="s">
-        <v>40</v>
-      </c>
-      <c r="V2" t="s">
-        <v>41</v>
-      </c>
-      <c r="W2" t="s">
-        <v>42</v>
-      </c>
-      <c r="X2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA2">
-        <v>28</v>
-      </c>
-      <c r="AB2">
-        <v>1200000</v>
-      </c>
-      <c r="AC2">
-        <v>3300000</v>
-      </c>
-      <c r="AD2">
-        <v>26.67</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>